<commit_message>
convert bitbuket to github
</commit_message>
<xml_diff>
--- a/src/main/webapp/data/Formlabel.xlsx
+++ b/src/main/webapp/data/Formlabel.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14475" windowHeight="4770" activeTab="1"/>
+    <workbookView xWindow="690" yWindow="690" windowWidth="14565" windowHeight="11820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Form xuat Excel(1)" sheetId="4" r:id="rId1"/>
     <sheet name="Form giao nhận(2)" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A7:I18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>No</t>
   </si>
@@ -37,15 +36,6 @@
   </si>
   <si>
     <t>UNIT</t>
-  </si>
-  <si>
-    <t>STOCK_TYPE</t>
-  </si>
-  <si>
-    <t>PRODUCTION_DATE</t>
-  </si>
-  <si>
-    <t>EXPIRE_DATE</t>
   </si>
   <si>
     <t>WO:</t>
@@ -100,16 +90,17 @@
   <si>
     <t>Ghi chú</t>
   </si>
+  <si>
+    <t>RECEIVING DATE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="165" formatCode="yy\-mm\-dd"/>
-    <numFmt numFmtId="166" formatCode="d/m/yy\ h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -483,7 +474,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -503,34 +494,6 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1418,48 +1381,48 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="38" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1562,69 +1525,69 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1650,48 +1613,48 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2167,48 +2130,48 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -2301,27 +2264,27 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2350,7 +2313,7 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2361,21 +2324,12 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2391,11 +2345,11 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2412,7 +2366,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2428,22 +2382,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1441">
     <cellStyle name="_200906SCHEDULE0519" xfId="3"/>
@@ -3918,22 +3872,34 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 1"/>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr>
           <a:grpSpLocks/>
         </xdr:cNvGrpSpPr>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4589611" y="7090040"/>
-          <a:ext cx="4049405" cy="665389"/>
+          <a:off x="4579423" y="7018730"/>
+          <a:ext cx="4056537" cy="665389"/>
           <a:chOff x="7924800" y="4724400"/>
           <a:chExt cx="3295650" cy="495300"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Rectangle 2"/>
+          <xdr:cNvPr id="3" name="Rectangle 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -3992,7 +3958,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Rectangle 3"/>
+          <xdr:cNvPr id="4" name="Rectangle 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -4048,7 +4020,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Rectangle 4"/>
+          <xdr:cNvPr id="5" name="Rectangle 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -4104,7 +4082,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="Rectangle 5"/>
+          <xdr:cNvPr id="6" name="Rectangle 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -4153,14 +4137,20 @@
                 <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
               </a:rPr>
-              <a:t>ZVF4-L054-01</a:t>
+              <a:t>ZVF4-L055-02</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7" name="Rectangle 6"/>
+          <xdr:cNvPr id="7" name="Rectangle 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -4207,14 +4197,20 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>25/9/2014</a:t>
+              <a:t>24/4/2015</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="Rectangle 7"/>
+          <xdr:cNvPr id="8" name="Rectangle 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -4270,7 +4266,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="9" name="Rectangle 8"/>
+          <xdr:cNvPr id="9" name="Rectangle 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -4317,14 +4319,20 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>1</a:t>
+              <a:t>3</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="Rectangle 9"/>
+          <xdr:cNvPr id="10" name="Rectangle 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -4371,14 +4379,20 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>1/6/2018</a:t>
+              <a:t>1/11/2019</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="11" name="TextBox 10"/>
+          <xdr:cNvPr id="11" name="TextBox 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -4427,33 +4441,45 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>69268</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>175153</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>295177</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1697182</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>96065</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="12" name="Group 11"/>
+        <xdr:cNvPr id="12" name="Group 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="0" y="6965918"/>
-          <a:ext cx="3365589" cy="1063912"/>
+          <a:off x="502223" y="6894608"/>
+          <a:ext cx="2528459" cy="1063912"/>
           <a:chOff x="7129" y="5046771"/>
-          <a:chExt cx="3359599" cy="1064712"/>
+          <a:chExt cx="2245718" cy="1064712"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="13" name="Rectangle 12"/>
+          <xdr:cNvPr id="13" name="Rectangle 12">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -4519,7 +4545,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="14" name="Rectangle 13"/>
+          <xdr:cNvPr id="14" name="Rectangle 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -4572,7 +4604,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="15" name="Rectangle 14"/>
+          <xdr:cNvPr id="15" name="Rectangle 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -4614,6 +4652,26 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
+              <a:rPr lang="en-US" sz="1000">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Người</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> trả (LL</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="vi-VN" sz="1000">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
@@ -4621,7 +4679,7 @@
                 <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
               </a:rPr>
-              <a:t>Xác nhận (KIT)</a:t>
+              <a:t>)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1000">
               <a:solidFill>
@@ -4635,132 +4693,19 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="16" name="Rectangle 15"/>
+          <xdr:cNvPr id="16" name="Rectangle 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
             <a:off x="1133043" y="5303096"/>
             <a:ext cx="1119804" cy="808387"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:sysClr val="window" lastClr="FFFFFF"/>
-          </a:solidFill>
-          <a:ln w="12700">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1000">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="17" name="Rectangle 16"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="2257275" y="5046771"/>
-            <a:ext cx="1109453" cy="260653"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:sysClr val="window" lastClr="FFFFFF"/>
-          </a:solidFill>
-          <a:ln w="12700">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="vi-VN" sz="1000">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
-                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
-              </a:rPr>
-              <a:t>Người trả</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1000">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
-                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
-              </a:rPr>
-              <a:t> (LL)</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="18" name="Rectangle 17"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="2257274" y="5309405"/>
-            <a:ext cx="1109454" cy="802078"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -5098,622 +5043,620 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:WVR107"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="17" style="6" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="6" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="10" style="6" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="16" style="6" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" style="6" hidden="1" customWidth="1"/>
-    <col min="11" max="256" width="9.140625" style="6"/>
-    <col min="257" max="257" width="7.28515625" style="6" customWidth="1"/>
-    <col min="258" max="258" width="17" style="6" customWidth="1"/>
-    <col min="259" max="259" width="25.28515625" style="6" customWidth="1"/>
-    <col min="260" max="260" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="8" style="6" customWidth="1"/>
-    <col min="262" max="262" width="18.85546875" style="6" customWidth="1"/>
-    <col min="263" max="263" width="7.28515625" style="6" customWidth="1"/>
-    <col min="264" max="266" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="267" max="512" width="9.140625" style="6"/>
-    <col min="513" max="513" width="7.28515625" style="6" customWidth="1"/>
-    <col min="514" max="514" width="17" style="6" customWidth="1"/>
-    <col min="515" max="515" width="25.28515625" style="6" customWidth="1"/>
-    <col min="516" max="516" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="517" max="517" width="8" style="6" customWidth="1"/>
-    <col min="518" max="518" width="18.85546875" style="6" customWidth="1"/>
-    <col min="519" max="519" width="7.28515625" style="6" customWidth="1"/>
-    <col min="520" max="522" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="523" max="768" width="9.140625" style="6"/>
-    <col min="769" max="769" width="7.28515625" style="6" customWidth="1"/>
-    <col min="770" max="770" width="17" style="6" customWidth="1"/>
-    <col min="771" max="771" width="25.28515625" style="6" customWidth="1"/>
-    <col min="772" max="772" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="773" max="773" width="8" style="6" customWidth="1"/>
-    <col min="774" max="774" width="18.85546875" style="6" customWidth="1"/>
-    <col min="775" max="775" width="7.28515625" style="6" customWidth="1"/>
-    <col min="776" max="778" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="779" max="1024" width="9.140625" style="6"/>
-    <col min="1025" max="1025" width="7.28515625" style="6" customWidth="1"/>
-    <col min="1026" max="1026" width="17" style="6" customWidth="1"/>
-    <col min="1027" max="1027" width="25.28515625" style="6" customWidth="1"/>
-    <col min="1028" max="1028" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="1029" max="1029" width="8" style="6" customWidth="1"/>
-    <col min="1030" max="1030" width="18.85546875" style="6" customWidth="1"/>
-    <col min="1031" max="1031" width="7.28515625" style="6" customWidth="1"/>
-    <col min="1032" max="1034" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="1035" max="1280" width="9.140625" style="6"/>
-    <col min="1281" max="1281" width="7.28515625" style="6" customWidth="1"/>
-    <col min="1282" max="1282" width="17" style="6" customWidth="1"/>
-    <col min="1283" max="1283" width="25.28515625" style="6" customWidth="1"/>
-    <col min="1284" max="1284" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="1285" max="1285" width="8" style="6" customWidth="1"/>
-    <col min="1286" max="1286" width="18.85546875" style="6" customWidth="1"/>
-    <col min="1287" max="1287" width="7.28515625" style="6" customWidth="1"/>
-    <col min="1288" max="1290" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="1291" max="1536" width="9.140625" style="6"/>
-    <col min="1537" max="1537" width="7.28515625" style="6" customWidth="1"/>
-    <col min="1538" max="1538" width="17" style="6" customWidth="1"/>
-    <col min="1539" max="1539" width="25.28515625" style="6" customWidth="1"/>
-    <col min="1540" max="1540" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="1541" max="1541" width="8" style="6" customWidth="1"/>
-    <col min="1542" max="1542" width="18.85546875" style="6" customWidth="1"/>
-    <col min="1543" max="1543" width="7.28515625" style="6" customWidth="1"/>
-    <col min="1544" max="1546" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="1547" max="1792" width="9.140625" style="6"/>
-    <col min="1793" max="1793" width="7.28515625" style="6" customWidth="1"/>
-    <col min="1794" max="1794" width="17" style="6" customWidth="1"/>
-    <col min="1795" max="1795" width="25.28515625" style="6" customWidth="1"/>
-    <col min="1796" max="1796" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="1797" max="1797" width="8" style="6" customWidth="1"/>
-    <col min="1798" max="1798" width="18.85546875" style="6" customWidth="1"/>
-    <col min="1799" max="1799" width="7.28515625" style="6" customWidth="1"/>
-    <col min="1800" max="1802" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="1803" max="2048" width="9.140625" style="6"/>
-    <col min="2049" max="2049" width="7.28515625" style="6" customWidth="1"/>
-    <col min="2050" max="2050" width="17" style="6" customWidth="1"/>
-    <col min="2051" max="2051" width="25.28515625" style="6" customWidth="1"/>
-    <col min="2052" max="2052" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2053" max="2053" width="8" style="6" customWidth="1"/>
-    <col min="2054" max="2054" width="18.85546875" style="6" customWidth="1"/>
-    <col min="2055" max="2055" width="7.28515625" style="6" customWidth="1"/>
-    <col min="2056" max="2058" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="2059" max="2304" width="9.140625" style="6"/>
-    <col min="2305" max="2305" width="7.28515625" style="6" customWidth="1"/>
-    <col min="2306" max="2306" width="17" style="6" customWidth="1"/>
-    <col min="2307" max="2307" width="25.28515625" style="6" customWidth="1"/>
-    <col min="2308" max="2308" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2309" max="2309" width="8" style="6" customWidth="1"/>
-    <col min="2310" max="2310" width="18.85546875" style="6" customWidth="1"/>
-    <col min="2311" max="2311" width="7.28515625" style="6" customWidth="1"/>
-    <col min="2312" max="2314" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="2315" max="2560" width="9.140625" style="6"/>
-    <col min="2561" max="2561" width="7.28515625" style="6" customWidth="1"/>
-    <col min="2562" max="2562" width="17" style="6" customWidth="1"/>
-    <col min="2563" max="2563" width="25.28515625" style="6" customWidth="1"/>
-    <col min="2564" max="2564" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2565" max="2565" width="8" style="6" customWidth="1"/>
-    <col min="2566" max="2566" width="18.85546875" style="6" customWidth="1"/>
-    <col min="2567" max="2567" width="7.28515625" style="6" customWidth="1"/>
-    <col min="2568" max="2570" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="2571" max="2816" width="9.140625" style="6"/>
-    <col min="2817" max="2817" width="7.28515625" style="6" customWidth="1"/>
-    <col min="2818" max="2818" width="17" style="6" customWidth="1"/>
-    <col min="2819" max="2819" width="25.28515625" style="6" customWidth="1"/>
-    <col min="2820" max="2820" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2821" max="2821" width="8" style="6" customWidth="1"/>
-    <col min="2822" max="2822" width="18.85546875" style="6" customWidth="1"/>
-    <col min="2823" max="2823" width="7.28515625" style="6" customWidth="1"/>
-    <col min="2824" max="2826" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="2827" max="3072" width="9.140625" style="6"/>
-    <col min="3073" max="3073" width="7.28515625" style="6" customWidth="1"/>
-    <col min="3074" max="3074" width="17" style="6" customWidth="1"/>
-    <col min="3075" max="3075" width="25.28515625" style="6" customWidth="1"/>
-    <col min="3076" max="3076" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3077" max="3077" width="8" style="6" customWidth="1"/>
-    <col min="3078" max="3078" width="18.85546875" style="6" customWidth="1"/>
-    <col min="3079" max="3079" width="7.28515625" style="6" customWidth="1"/>
-    <col min="3080" max="3082" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="3083" max="3328" width="9.140625" style="6"/>
-    <col min="3329" max="3329" width="7.28515625" style="6" customWidth="1"/>
-    <col min="3330" max="3330" width="17" style="6" customWidth="1"/>
-    <col min="3331" max="3331" width="25.28515625" style="6" customWidth="1"/>
-    <col min="3332" max="3332" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3333" max="3333" width="8" style="6" customWidth="1"/>
-    <col min="3334" max="3334" width="18.85546875" style="6" customWidth="1"/>
-    <col min="3335" max="3335" width="7.28515625" style="6" customWidth="1"/>
-    <col min="3336" max="3338" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="3339" max="3584" width="9.140625" style="6"/>
-    <col min="3585" max="3585" width="7.28515625" style="6" customWidth="1"/>
-    <col min="3586" max="3586" width="17" style="6" customWidth="1"/>
-    <col min="3587" max="3587" width="25.28515625" style="6" customWidth="1"/>
-    <col min="3588" max="3588" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3589" max="3589" width="8" style="6" customWidth="1"/>
-    <col min="3590" max="3590" width="18.85546875" style="6" customWidth="1"/>
-    <col min="3591" max="3591" width="7.28515625" style="6" customWidth="1"/>
-    <col min="3592" max="3594" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="3595" max="3840" width="9.140625" style="6"/>
-    <col min="3841" max="3841" width="7.28515625" style="6" customWidth="1"/>
-    <col min="3842" max="3842" width="17" style="6" customWidth="1"/>
-    <col min="3843" max="3843" width="25.28515625" style="6" customWidth="1"/>
-    <col min="3844" max="3844" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3845" max="3845" width="8" style="6" customWidth="1"/>
-    <col min="3846" max="3846" width="18.85546875" style="6" customWidth="1"/>
-    <col min="3847" max="3847" width="7.28515625" style="6" customWidth="1"/>
-    <col min="3848" max="3850" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="3851" max="4096" width="9.140625" style="6"/>
-    <col min="4097" max="4097" width="7.28515625" style="6" customWidth="1"/>
-    <col min="4098" max="4098" width="17" style="6" customWidth="1"/>
-    <col min="4099" max="4099" width="25.28515625" style="6" customWidth="1"/>
-    <col min="4100" max="4100" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4101" max="4101" width="8" style="6" customWidth="1"/>
-    <col min="4102" max="4102" width="18.85546875" style="6" customWidth="1"/>
-    <col min="4103" max="4103" width="7.28515625" style="6" customWidth="1"/>
-    <col min="4104" max="4106" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="4107" max="4352" width="9.140625" style="6"/>
-    <col min="4353" max="4353" width="7.28515625" style="6" customWidth="1"/>
-    <col min="4354" max="4354" width="17" style="6" customWidth="1"/>
-    <col min="4355" max="4355" width="25.28515625" style="6" customWidth="1"/>
-    <col min="4356" max="4356" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4357" max="4357" width="8" style="6" customWidth="1"/>
-    <col min="4358" max="4358" width="18.85546875" style="6" customWidth="1"/>
-    <col min="4359" max="4359" width="7.28515625" style="6" customWidth="1"/>
-    <col min="4360" max="4362" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="4363" max="4608" width="9.140625" style="6"/>
-    <col min="4609" max="4609" width="7.28515625" style="6" customWidth="1"/>
-    <col min="4610" max="4610" width="17" style="6" customWidth="1"/>
-    <col min="4611" max="4611" width="25.28515625" style="6" customWidth="1"/>
-    <col min="4612" max="4612" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4613" max="4613" width="8" style="6" customWidth="1"/>
-    <col min="4614" max="4614" width="18.85546875" style="6" customWidth="1"/>
-    <col min="4615" max="4615" width="7.28515625" style="6" customWidth="1"/>
-    <col min="4616" max="4618" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="4619" max="4864" width="9.140625" style="6"/>
-    <col min="4865" max="4865" width="7.28515625" style="6" customWidth="1"/>
-    <col min="4866" max="4866" width="17" style="6" customWidth="1"/>
-    <col min="4867" max="4867" width="25.28515625" style="6" customWidth="1"/>
-    <col min="4868" max="4868" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4869" max="4869" width="8" style="6" customWidth="1"/>
-    <col min="4870" max="4870" width="18.85546875" style="6" customWidth="1"/>
-    <col min="4871" max="4871" width="7.28515625" style="6" customWidth="1"/>
-    <col min="4872" max="4874" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="4875" max="5120" width="9.140625" style="6"/>
-    <col min="5121" max="5121" width="7.28515625" style="6" customWidth="1"/>
-    <col min="5122" max="5122" width="17" style="6" customWidth="1"/>
-    <col min="5123" max="5123" width="25.28515625" style="6" customWidth="1"/>
-    <col min="5124" max="5124" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5125" max="5125" width="8" style="6" customWidth="1"/>
-    <col min="5126" max="5126" width="18.85546875" style="6" customWidth="1"/>
-    <col min="5127" max="5127" width="7.28515625" style="6" customWidth="1"/>
-    <col min="5128" max="5130" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="5131" max="5376" width="9.140625" style="6"/>
-    <col min="5377" max="5377" width="7.28515625" style="6" customWidth="1"/>
-    <col min="5378" max="5378" width="17" style="6" customWidth="1"/>
-    <col min="5379" max="5379" width="25.28515625" style="6" customWidth="1"/>
-    <col min="5380" max="5380" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5381" max="5381" width="8" style="6" customWidth="1"/>
-    <col min="5382" max="5382" width="18.85546875" style="6" customWidth="1"/>
-    <col min="5383" max="5383" width="7.28515625" style="6" customWidth="1"/>
-    <col min="5384" max="5386" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="5387" max="5632" width="9.140625" style="6"/>
-    <col min="5633" max="5633" width="7.28515625" style="6" customWidth="1"/>
-    <col min="5634" max="5634" width="17" style="6" customWidth="1"/>
-    <col min="5635" max="5635" width="25.28515625" style="6" customWidth="1"/>
-    <col min="5636" max="5636" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5637" max="5637" width="8" style="6" customWidth="1"/>
-    <col min="5638" max="5638" width="18.85546875" style="6" customWidth="1"/>
-    <col min="5639" max="5639" width="7.28515625" style="6" customWidth="1"/>
-    <col min="5640" max="5642" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="5643" max="5888" width="9.140625" style="6"/>
-    <col min="5889" max="5889" width="7.28515625" style="6" customWidth="1"/>
-    <col min="5890" max="5890" width="17" style="6" customWidth="1"/>
-    <col min="5891" max="5891" width="25.28515625" style="6" customWidth="1"/>
-    <col min="5892" max="5892" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5893" max="5893" width="8" style="6" customWidth="1"/>
-    <col min="5894" max="5894" width="18.85546875" style="6" customWidth="1"/>
-    <col min="5895" max="5895" width="7.28515625" style="6" customWidth="1"/>
-    <col min="5896" max="5898" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="5899" max="6144" width="9.140625" style="6"/>
-    <col min="6145" max="6145" width="7.28515625" style="6" customWidth="1"/>
-    <col min="6146" max="6146" width="17" style="6" customWidth="1"/>
-    <col min="6147" max="6147" width="25.28515625" style="6" customWidth="1"/>
-    <col min="6148" max="6148" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6149" max="6149" width="8" style="6" customWidth="1"/>
-    <col min="6150" max="6150" width="18.85546875" style="6" customWidth="1"/>
-    <col min="6151" max="6151" width="7.28515625" style="6" customWidth="1"/>
-    <col min="6152" max="6154" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="6155" max="6400" width="9.140625" style="6"/>
-    <col min="6401" max="6401" width="7.28515625" style="6" customWidth="1"/>
-    <col min="6402" max="6402" width="17" style="6" customWidth="1"/>
-    <col min="6403" max="6403" width="25.28515625" style="6" customWidth="1"/>
-    <col min="6404" max="6404" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6405" max="6405" width="8" style="6" customWidth="1"/>
-    <col min="6406" max="6406" width="18.85546875" style="6" customWidth="1"/>
-    <col min="6407" max="6407" width="7.28515625" style="6" customWidth="1"/>
-    <col min="6408" max="6410" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="6411" max="6656" width="9.140625" style="6"/>
-    <col min="6657" max="6657" width="7.28515625" style="6" customWidth="1"/>
-    <col min="6658" max="6658" width="17" style="6" customWidth="1"/>
-    <col min="6659" max="6659" width="25.28515625" style="6" customWidth="1"/>
-    <col min="6660" max="6660" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6661" max="6661" width="8" style="6" customWidth="1"/>
-    <col min="6662" max="6662" width="18.85546875" style="6" customWidth="1"/>
-    <col min="6663" max="6663" width="7.28515625" style="6" customWidth="1"/>
-    <col min="6664" max="6666" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="6667" max="6912" width="9.140625" style="6"/>
-    <col min="6913" max="6913" width="7.28515625" style="6" customWidth="1"/>
-    <col min="6914" max="6914" width="17" style="6" customWidth="1"/>
-    <col min="6915" max="6915" width="25.28515625" style="6" customWidth="1"/>
-    <col min="6916" max="6916" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6917" max="6917" width="8" style="6" customWidth="1"/>
-    <col min="6918" max="6918" width="18.85546875" style="6" customWidth="1"/>
-    <col min="6919" max="6919" width="7.28515625" style="6" customWidth="1"/>
-    <col min="6920" max="6922" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="6923" max="7168" width="9.140625" style="6"/>
-    <col min="7169" max="7169" width="7.28515625" style="6" customWidth="1"/>
-    <col min="7170" max="7170" width="17" style="6" customWidth="1"/>
-    <col min="7171" max="7171" width="25.28515625" style="6" customWidth="1"/>
-    <col min="7172" max="7172" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7173" max="7173" width="8" style="6" customWidth="1"/>
-    <col min="7174" max="7174" width="18.85546875" style="6" customWidth="1"/>
-    <col min="7175" max="7175" width="7.28515625" style="6" customWidth="1"/>
-    <col min="7176" max="7178" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="7179" max="7424" width="9.140625" style="6"/>
-    <col min="7425" max="7425" width="7.28515625" style="6" customWidth="1"/>
-    <col min="7426" max="7426" width="17" style="6" customWidth="1"/>
-    <col min="7427" max="7427" width="25.28515625" style="6" customWidth="1"/>
-    <col min="7428" max="7428" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7429" max="7429" width="8" style="6" customWidth="1"/>
-    <col min="7430" max="7430" width="18.85546875" style="6" customWidth="1"/>
-    <col min="7431" max="7431" width="7.28515625" style="6" customWidth="1"/>
-    <col min="7432" max="7434" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="7435" max="7680" width="9.140625" style="6"/>
-    <col min="7681" max="7681" width="7.28515625" style="6" customWidth="1"/>
-    <col min="7682" max="7682" width="17" style="6" customWidth="1"/>
-    <col min="7683" max="7683" width="25.28515625" style="6" customWidth="1"/>
-    <col min="7684" max="7684" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7685" max="7685" width="8" style="6" customWidth="1"/>
-    <col min="7686" max="7686" width="18.85546875" style="6" customWidth="1"/>
-    <col min="7687" max="7687" width="7.28515625" style="6" customWidth="1"/>
-    <col min="7688" max="7690" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="7691" max="7936" width="9.140625" style="6"/>
-    <col min="7937" max="7937" width="7.28515625" style="6" customWidth="1"/>
-    <col min="7938" max="7938" width="17" style="6" customWidth="1"/>
-    <col min="7939" max="7939" width="25.28515625" style="6" customWidth="1"/>
-    <col min="7940" max="7940" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7941" max="7941" width="8" style="6" customWidth="1"/>
-    <col min="7942" max="7942" width="18.85546875" style="6" customWidth="1"/>
-    <col min="7943" max="7943" width="7.28515625" style="6" customWidth="1"/>
-    <col min="7944" max="7946" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="7947" max="8192" width="9.140625" style="6"/>
-    <col min="8193" max="8193" width="7.28515625" style="6" customWidth="1"/>
-    <col min="8194" max="8194" width="17" style="6" customWidth="1"/>
-    <col min="8195" max="8195" width="25.28515625" style="6" customWidth="1"/>
-    <col min="8196" max="8196" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8197" max="8197" width="8" style="6" customWidth="1"/>
-    <col min="8198" max="8198" width="18.85546875" style="6" customWidth="1"/>
-    <col min="8199" max="8199" width="7.28515625" style="6" customWidth="1"/>
-    <col min="8200" max="8202" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="8203" max="8448" width="9.140625" style="6"/>
-    <col min="8449" max="8449" width="7.28515625" style="6" customWidth="1"/>
-    <col min="8450" max="8450" width="17" style="6" customWidth="1"/>
-    <col min="8451" max="8451" width="25.28515625" style="6" customWidth="1"/>
-    <col min="8452" max="8452" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8453" max="8453" width="8" style="6" customWidth="1"/>
-    <col min="8454" max="8454" width="18.85546875" style="6" customWidth="1"/>
-    <col min="8455" max="8455" width="7.28515625" style="6" customWidth="1"/>
-    <col min="8456" max="8458" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="8459" max="8704" width="9.140625" style="6"/>
-    <col min="8705" max="8705" width="7.28515625" style="6" customWidth="1"/>
-    <col min="8706" max="8706" width="17" style="6" customWidth="1"/>
-    <col min="8707" max="8707" width="25.28515625" style="6" customWidth="1"/>
-    <col min="8708" max="8708" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8709" max="8709" width="8" style="6" customWidth="1"/>
-    <col min="8710" max="8710" width="18.85546875" style="6" customWidth="1"/>
-    <col min="8711" max="8711" width="7.28515625" style="6" customWidth="1"/>
-    <col min="8712" max="8714" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="8715" max="8960" width="9.140625" style="6"/>
-    <col min="8961" max="8961" width="7.28515625" style="6" customWidth="1"/>
-    <col min="8962" max="8962" width="17" style="6" customWidth="1"/>
-    <col min="8963" max="8963" width="25.28515625" style="6" customWidth="1"/>
-    <col min="8964" max="8964" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8965" max="8965" width="8" style="6" customWidth="1"/>
-    <col min="8966" max="8966" width="18.85546875" style="6" customWidth="1"/>
-    <col min="8967" max="8967" width="7.28515625" style="6" customWidth="1"/>
-    <col min="8968" max="8970" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="8971" max="9216" width="9.140625" style="6"/>
-    <col min="9217" max="9217" width="7.28515625" style="6" customWidth="1"/>
-    <col min="9218" max="9218" width="17" style="6" customWidth="1"/>
-    <col min="9219" max="9219" width="25.28515625" style="6" customWidth="1"/>
-    <col min="9220" max="9220" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9221" max="9221" width="8" style="6" customWidth="1"/>
-    <col min="9222" max="9222" width="18.85546875" style="6" customWidth="1"/>
-    <col min="9223" max="9223" width="7.28515625" style="6" customWidth="1"/>
-    <col min="9224" max="9226" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="9227" max="9472" width="9.140625" style="6"/>
-    <col min="9473" max="9473" width="7.28515625" style="6" customWidth="1"/>
-    <col min="9474" max="9474" width="17" style="6" customWidth="1"/>
-    <col min="9475" max="9475" width="25.28515625" style="6" customWidth="1"/>
-    <col min="9476" max="9476" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9477" max="9477" width="8" style="6" customWidth="1"/>
-    <col min="9478" max="9478" width="18.85546875" style="6" customWidth="1"/>
-    <col min="9479" max="9479" width="7.28515625" style="6" customWidth="1"/>
-    <col min="9480" max="9482" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="9483" max="9728" width="9.140625" style="6"/>
-    <col min="9729" max="9729" width="7.28515625" style="6" customWidth="1"/>
-    <col min="9730" max="9730" width="17" style="6" customWidth="1"/>
-    <col min="9731" max="9731" width="25.28515625" style="6" customWidth="1"/>
-    <col min="9732" max="9732" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9733" max="9733" width="8" style="6" customWidth="1"/>
-    <col min="9734" max="9734" width="18.85546875" style="6" customWidth="1"/>
-    <col min="9735" max="9735" width="7.28515625" style="6" customWidth="1"/>
-    <col min="9736" max="9738" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="9739" max="9984" width="9.140625" style="6"/>
-    <col min="9985" max="9985" width="7.28515625" style="6" customWidth="1"/>
-    <col min="9986" max="9986" width="17" style="6" customWidth="1"/>
-    <col min="9987" max="9987" width="25.28515625" style="6" customWidth="1"/>
-    <col min="9988" max="9988" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9989" max="9989" width="8" style="6" customWidth="1"/>
-    <col min="9990" max="9990" width="18.85546875" style="6" customWidth="1"/>
-    <col min="9991" max="9991" width="7.28515625" style="6" customWidth="1"/>
-    <col min="9992" max="9994" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="9995" max="10240" width="9.140625" style="6"/>
-    <col min="10241" max="10241" width="7.28515625" style="6" customWidth="1"/>
-    <col min="10242" max="10242" width="17" style="6" customWidth="1"/>
-    <col min="10243" max="10243" width="25.28515625" style="6" customWidth="1"/>
-    <col min="10244" max="10244" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10245" max="10245" width="8" style="6" customWidth="1"/>
-    <col min="10246" max="10246" width="18.85546875" style="6" customWidth="1"/>
-    <col min="10247" max="10247" width="7.28515625" style="6" customWidth="1"/>
-    <col min="10248" max="10250" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="10251" max="10496" width="9.140625" style="6"/>
-    <col min="10497" max="10497" width="7.28515625" style="6" customWidth="1"/>
-    <col min="10498" max="10498" width="17" style="6" customWidth="1"/>
-    <col min="10499" max="10499" width="25.28515625" style="6" customWidth="1"/>
-    <col min="10500" max="10500" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10501" max="10501" width="8" style="6" customWidth="1"/>
-    <col min="10502" max="10502" width="18.85546875" style="6" customWidth="1"/>
-    <col min="10503" max="10503" width="7.28515625" style="6" customWidth="1"/>
-    <col min="10504" max="10506" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="10507" max="10752" width="9.140625" style="6"/>
-    <col min="10753" max="10753" width="7.28515625" style="6" customWidth="1"/>
-    <col min="10754" max="10754" width="17" style="6" customWidth="1"/>
-    <col min="10755" max="10755" width="25.28515625" style="6" customWidth="1"/>
-    <col min="10756" max="10756" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10757" max="10757" width="8" style="6" customWidth="1"/>
-    <col min="10758" max="10758" width="18.85546875" style="6" customWidth="1"/>
-    <col min="10759" max="10759" width="7.28515625" style="6" customWidth="1"/>
-    <col min="10760" max="10762" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="10763" max="11008" width="9.140625" style="6"/>
-    <col min="11009" max="11009" width="7.28515625" style="6" customWidth="1"/>
-    <col min="11010" max="11010" width="17" style="6" customWidth="1"/>
-    <col min="11011" max="11011" width="25.28515625" style="6" customWidth="1"/>
-    <col min="11012" max="11012" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11013" max="11013" width="8" style="6" customWidth="1"/>
-    <col min="11014" max="11014" width="18.85546875" style="6" customWidth="1"/>
-    <col min="11015" max="11015" width="7.28515625" style="6" customWidth="1"/>
-    <col min="11016" max="11018" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="11019" max="11264" width="9.140625" style="6"/>
-    <col min="11265" max="11265" width="7.28515625" style="6" customWidth="1"/>
-    <col min="11266" max="11266" width="17" style="6" customWidth="1"/>
-    <col min="11267" max="11267" width="25.28515625" style="6" customWidth="1"/>
-    <col min="11268" max="11268" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11269" max="11269" width="8" style="6" customWidth="1"/>
-    <col min="11270" max="11270" width="18.85546875" style="6" customWidth="1"/>
-    <col min="11271" max="11271" width="7.28515625" style="6" customWidth="1"/>
-    <col min="11272" max="11274" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="11275" max="11520" width="9.140625" style="6"/>
-    <col min="11521" max="11521" width="7.28515625" style="6" customWidth="1"/>
-    <col min="11522" max="11522" width="17" style="6" customWidth="1"/>
-    <col min="11523" max="11523" width="25.28515625" style="6" customWidth="1"/>
-    <col min="11524" max="11524" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11525" max="11525" width="8" style="6" customWidth="1"/>
-    <col min="11526" max="11526" width="18.85546875" style="6" customWidth="1"/>
-    <col min="11527" max="11527" width="7.28515625" style="6" customWidth="1"/>
-    <col min="11528" max="11530" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="11531" max="11776" width="9.140625" style="6"/>
-    <col min="11777" max="11777" width="7.28515625" style="6" customWidth="1"/>
-    <col min="11778" max="11778" width="17" style="6" customWidth="1"/>
-    <col min="11779" max="11779" width="25.28515625" style="6" customWidth="1"/>
-    <col min="11780" max="11780" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11781" max="11781" width="8" style="6" customWidth="1"/>
-    <col min="11782" max="11782" width="18.85546875" style="6" customWidth="1"/>
-    <col min="11783" max="11783" width="7.28515625" style="6" customWidth="1"/>
-    <col min="11784" max="11786" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="11787" max="12032" width="9.140625" style="6"/>
-    <col min="12033" max="12033" width="7.28515625" style="6" customWidth="1"/>
-    <col min="12034" max="12034" width="17" style="6" customWidth="1"/>
-    <col min="12035" max="12035" width="25.28515625" style="6" customWidth="1"/>
-    <col min="12036" max="12036" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12037" max="12037" width="8" style="6" customWidth="1"/>
-    <col min="12038" max="12038" width="18.85546875" style="6" customWidth="1"/>
-    <col min="12039" max="12039" width="7.28515625" style="6" customWidth="1"/>
-    <col min="12040" max="12042" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="12043" max="12288" width="9.140625" style="6"/>
-    <col min="12289" max="12289" width="7.28515625" style="6" customWidth="1"/>
-    <col min="12290" max="12290" width="17" style="6" customWidth="1"/>
-    <col min="12291" max="12291" width="25.28515625" style="6" customWidth="1"/>
-    <col min="12292" max="12292" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12293" max="12293" width="8" style="6" customWidth="1"/>
-    <col min="12294" max="12294" width="18.85546875" style="6" customWidth="1"/>
-    <col min="12295" max="12295" width="7.28515625" style="6" customWidth="1"/>
-    <col min="12296" max="12298" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="12299" max="12544" width="9.140625" style="6"/>
-    <col min="12545" max="12545" width="7.28515625" style="6" customWidth="1"/>
-    <col min="12546" max="12546" width="17" style="6" customWidth="1"/>
-    <col min="12547" max="12547" width="25.28515625" style="6" customWidth="1"/>
-    <col min="12548" max="12548" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12549" max="12549" width="8" style="6" customWidth="1"/>
-    <col min="12550" max="12550" width="18.85546875" style="6" customWidth="1"/>
-    <col min="12551" max="12551" width="7.28515625" style="6" customWidth="1"/>
-    <col min="12552" max="12554" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="12555" max="12800" width="9.140625" style="6"/>
-    <col min="12801" max="12801" width="7.28515625" style="6" customWidth="1"/>
-    <col min="12802" max="12802" width="17" style="6" customWidth="1"/>
-    <col min="12803" max="12803" width="25.28515625" style="6" customWidth="1"/>
-    <col min="12804" max="12804" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12805" max="12805" width="8" style="6" customWidth="1"/>
-    <col min="12806" max="12806" width="18.85546875" style="6" customWidth="1"/>
-    <col min="12807" max="12807" width="7.28515625" style="6" customWidth="1"/>
-    <col min="12808" max="12810" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="12811" max="13056" width="9.140625" style="6"/>
-    <col min="13057" max="13057" width="7.28515625" style="6" customWidth="1"/>
-    <col min="13058" max="13058" width="17" style="6" customWidth="1"/>
-    <col min="13059" max="13059" width="25.28515625" style="6" customWidth="1"/>
-    <col min="13060" max="13060" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13061" max="13061" width="8" style="6" customWidth="1"/>
-    <col min="13062" max="13062" width="18.85546875" style="6" customWidth="1"/>
-    <col min="13063" max="13063" width="7.28515625" style="6" customWidth="1"/>
-    <col min="13064" max="13066" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="13067" max="13312" width="9.140625" style="6"/>
-    <col min="13313" max="13313" width="7.28515625" style="6" customWidth="1"/>
-    <col min="13314" max="13314" width="17" style="6" customWidth="1"/>
-    <col min="13315" max="13315" width="25.28515625" style="6" customWidth="1"/>
-    <col min="13316" max="13316" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13317" max="13317" width="8" style="6" customWidth="1"/>
-    <col min="13318" max="13318" width="18.85546875" style="6" customWidth="1"/>
-    <col min="13319" max="13319" width="7.28515625" style="6" customWidth="1"/>
-    <col min="13320" max="13322" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="13323" max="13568" width="9.140625" style="6"/>
-    <col min="13569" max="13569" width="7.28515625" style="6" customWidth="1"/>
-    <col min="13570" max="13570" width="17" style="6" customWidth="1"/>
-    <col min="13571" max="13571" width="25.28515625" style="6" customWidth="1"/>
-    <col min="13572" max="13572" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13573" max="13573" width="8" style="6" customWidth="1"/>
-    <col min="13574" max="13574" width="18.85546875" style="6" customWidth="1"/>
-    <col min="13575" max="13575" width="7.28515625" style="6" customWidth="1"/>
-    <col min="13576" max="13578" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="13579" max="13824" width="9.140625" style="6"/>
-    <col min="13825" max="13825" width="7.28515625" style="6" customWidth="1"/>
-    <col min="13826" max="13826" width="17" style="6" customWidth="1"/>
-    <col min="13827" max="13827" width="25.28515625" style="6" customWidth="1"/>
-    <col min="13828" max="13828" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13829" max="13829" width="8" style="6" customWidth="1"/>
-    <col min="13830" max="13830" width="18.85546875" style="6" customWidth="1"/>
-    <col min="13831" max="13831" width="7.28515625" style="6" customWidth="1"/>
-    <col min="13832" max="13834" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="13835" max="14080" width="9.140625" style="6"/>
-    <col min="14081" max="14081" width="7.28515625" style="6" customWidth="1"/>
-    <col min="14082" max="14082" width="17" style="6" customWidth="1"/>
-    <col min="14083" max="14083" width="25.28515625" style="6" customWidth="1"/>
-    <col min="14084" max="14084" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14085" max="14085" width="8" style="6" customWidth="1"/>
-    <col min="14086" max="14086" width="18.85546875" style="6" customWidth="1"/>
-    <col min="14087" max="14087" width="7.28515625" style="6" customWidth="1"/>
-    <col min="14088" max="14090" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="14091" max="14336" width="9.140625" style="6"/>
-    <col min="14337" max="14337" width="7.28515625" style="6" customWidth="1"/>
-    <col min="14338" max="14338" width="17" style="6" customWidth="1"/>
-    <col min="14339" max="14339" width="25.28515625" style="6" customWidth="1"/>
-    <col min="14340" max="14340" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14341" max="14341" width="8" style="6" customWidth="1"/>
-    <col min="14342" max="14342" width="18.85546875" style="6" customWidth="1"/>
-    <col min="14343" max="14343" width="7.28515625" style="6" customWidth="1"/>
-    <col min="14344" max="14346" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="14347" max="14592" width="9.140625" style="6"/>
-    <col min="14593" max="14593" width="7.28515625" style="6" customWidth="1"/>
-    <col min="14594" max="14594" width="17" style="6" customWidth="1"/>
-    <col min="14595" max="14595" width="25.28515625" style="6" customWidth="1"/>
-    <col min="14596" max="14596" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14597" max="14597" width="8" style="6" customWidth="1"/>
-    <col min="14598" max="14598" width="18.85546875" style="6" customWidth="1"/>
-    <col min="14599" max="14599" width="7.28515625" style="6" customWidth="1"/>
-    <col min="14600" max="14602" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="14603" max="14848" width="9.140625" style="6"/>
-    <col min="14849" max="14849" width="7.28515625" style="6" customWidth="1"/>
-    <col min="14850" max="14850" width="17" style="6" customWidth="1"/>
-    <col min="14851" max="14851" width="25.28515625" style="6" customWidth="1"/>
-    <col min="14852" max="14852" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14853" max="14853" width="8" style="6" customWidth="1"/>
-    <col min="14854" max="14854" width="18.85546875" style="6" customWidth="1"/>
-    <col min="14855" max="14855" width="7.28515625" style="6" customWidth="1"/>
-    <col min="14856" max="14858" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="14859" max="15104" width="9.140625" style="6"/>
-    <col min="15105" max="15105" width="7.28515625" style="6" customWidth="1"/>
-    <col min="15106" max="15106" width="17" style="6" customWidth="1"/>
-    <col min="15107" max="15107" width="25.28515625" style="6" customWidth="1"/>
-    <col min="15108" max="15108" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15109" max="15109" width="8" style="6" customWidth="1"/>
-    <col min="15110" max="15110" width="18.85546875" style="6" customWidth="1"/>
-    <col min="15111" max="15111" width="7.28515625" style="6" customWidth="1"/>
-    <col min="15112" max="15114" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="15115" max="15360" width="9.140625" style="6"/>
-    <col min="15361" max="15361" width="7.28515625" style="6" customWidth="1"/>
-    <col min="15362" max="15362" width="17" style="6" customWidth="1"/>
-    <col min="15363" max="15363" width="25.28515625" style="6" customWidth="1"/>
-    <col min="15364" max="15364" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15365" max="15365" width="8" style="6" customWidth="1"/>
-    <col min="15366" max="15366" width="18.85546875" style="6" customWidth="1"/>
-    <col min="15367" max="15367" width="7.28515625" style="6" customWidth="1"/>
-    <col min="15368" max="15370" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="15371" max="15616" width="9.140625" style="6"/>
-    <col min="15617" max="15617" width="7.28515625" style="6" customWidth="1"/>
-    <col min="15618" max="15618" width="17" style="6" customWidth="1"/>
-    <col min="15619" max="15619" width="25.28515625" style="6" customWidth="1"/>
-    <col min="15620" max="15620" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15621" max="15621" width="8" style="6" customWidth="1"/>
-    <col min="15622" max="15622" width="18.85546875" style="6" customWidth="1"/>
-    <col min="15623" max="15623" width="7.28515625" style="6" customWidth="1"/>
-    <col min="15624" max="15626" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="15627" max="15872" width="9.140625" style="6"/>
-    <col min="15873" max="15873" width="7.28515625" style="6" customWidth="1"/>
-    <col min="15874" max="15874" width="17" style="6" customWidth="1"/>
-    <col min="15875" max="15875" width="25.28515625" style="6" customWidth="1"/>
-    <col min="15876" max="15876" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15877" max="15877" width="8" style="6" customWidth="1"/>
-    <col min="15878" max="15878" width="18.85546875" style="6" customWidth="1"/>
-    <col min="15879" max="15879" width="7.28515625" style="6" customWidth="1"/>
-    <col min="15880" max="15882" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="15883" max="16128" width="9.140625" style="6"/>
-    <col min="16129" max="16129" width="7.28515625" style="6" customWidth="1"/>
-    <col min="16130" max="16130" width="17" style="6" customWidth="1"/>
-    <col min="16131" max="16131" width="25.28515625" style="6" customWidth="1"/>
-    <col min="16132" max="16132" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="16133" max="16133" width="8" style="6" customWidth="1"/>
-    <col min="16134" max="16134" width="18.85546875" style="6" customWidth="1"/>
-    <col min="16135" max="16135" width="7.28515625" style="6" customWidth="1"/>
-    <col min="16136" max="16138" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="16139" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="7.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17" style="4" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="18" style="4" customWidth="1"/>
+    <col min="9" max="253" width="9.140625" style="4"/>
+    <col min="254" max="254" width="7.28515625" style="4" customWidth="1"/>
+    <col min="255" max="255" width="17" style="4" customWidth="1"/>
+    <col min="256" max="256" width="25.28515625" style="4" customWidth="1"/>
+    <col min="257" max="257" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="8" style="4" customWidth="1"/>
+    <col min="259" max="259" width="18.85546875" style="4" customWidth="1"/>
+    <col min="260" max="260" width="7.28515625" style="4" customWidth="1"/>
+    <col min="261" max="263" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="264" max="509" width="9.140625" style="4"/>
+    <col min="510" max="510" width="7.28515625" style="4" customWidth="1"/>
+    <col min="511" max="511" width="17" style="4" customWidth="1"/>
+    <col min="512" max="512" width="25.28515625" style="4" customWidth="1"/>
+    <col min="513" max="513" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="8" style="4" customWidth="1"/>
+    <col min="515" max="515" width="18.85546875" style="4" customWidth="1"/>
+    <col min="516" max="516" width="7.28515625" style="4" customWidth="1"/>
+    <col min="517" max="519" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="520" max="765" width="9.140625" style="4"/>
+    <col min="766" max="766" width="7.28515625" style="4" customWidth="1"/>
+    <col min="767" max="767" width="17" style="4" customWidth="1"/>
+    <col min="768" max="768" width="25.28515625" style="4" customWidth="1"/>
+    <col min="769" max="769" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="8" style="4" customWidth="1"/>
+    <col min="771" max="771" width="18.85546875" style="4" customWidth="1"/>
+    <col min="772" max="772" width="7.28515625" style="4" customWidth="1"/>
+    <col min="773" max="775" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="776" max="1021" width="9.140625" style="4"/>
+    <col min="1022" max="1022" width="7.28515625" style="4" customWidth="1"/>
+    <col min="1023" max="1023" width="17" style="4" customWidth="1"/>
+    <col min="1024" max="1024" width="25.28515625" style="4" customWidth="1"/>
+    <col min="1025" max="1025" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="8" style="4" customWidth="1"/>
+    <col min="1027" max="1027" width="18.85546875" style="4" customWidth="1"/>
+    <col min="1028" max="1028" width="7.28515625" style="4" customWidth="1"/>
+    <col min="1029" max="1031" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="1032" max="1277" width="9.140625" style="4"/>
+    <col min="1278" max="1278" width="7.28515625" style="4" customWidth="1"/>
+    <col min="1279" max="1279" width="17" style="4" customWidth="1"/>
+    <col min="1280" max="1280" width="25.28515625" style="4" customWidth="1"/>
+    <col min="1281" max="1281" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="8" style="4" customWidth="1"/>
+    <col min="1283" max="1283" width="18.85546875" style="4" customWidth="1"/>
+    <col min="1284" max="1284" width="7.28515625" style="4" customWidth="1"/>
+    <col min="1285" max="1287" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="1288" max="1533" width="9.140625" style="4"/>
+    <col min="1534" max="1534" width="7.28515625" style="4" customWidth="1"/>
+    <col min="1535" max="1535" width="17" style="4" customWidth="1"/>
+    <col min="1536" max="1536" width="25.28515625" style="4" customWidth="1"/>
+    <col min="1537" max="1537" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="8" style="4" customWidth="1"/>
+    <col min="1539" max="1539" width="18.85546875" style="4" customWidth="1"/>
+    <col min="1540" max="1540" width="7.28515625" style="4" customWidth="1"/>
+    <col min="1541" max="1543" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="1544" max="1789" width="9.140625" style="4"/>
+    <col min="1790" max="1790" width="7.28515625" style="4" customWidth="1"/>
+    <col min="1791" max="1791" width="17" style="4" customWidth="1"/>
+    <col min="1792" max="1792" width="25.28515625" style="4" customWidth="1"/>
+    <col min="1793" max="1793" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="8" style="4" customWidth="1"/>
+    <col min="1795" max="1795" width="18.85546875" style="4" customWidth="1"/>
+    <col min="1796" max="1796" width="7.28515625" style="4" customWidth="1"/>
+    <col min="1797" max="1799" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="1800" max="2045" width="9.140625" style="4"/>
+    <col min="2046" max="2046" width="7.28515625" style="4" customWidth="1"/>
+    <col min="2047" max="2047" width="17" style="4" customWidth="1"/>
+    <col min="2048" max="2048" width="25.28515625" style="4" customWidth="1"/>
+    <col min="2049" max="2049" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="8" style="4" customWidth="1"/>
+    <col min="2051" max="2051" width="18.85546875" style="4" customWidth="1"/>
+    <col min="2052" max="2052" width="7.28515625" style="4" customWidth="1"/>
+    <col min="2053" max="2055" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="2056" max="2301" width="9.140625" style="4"/>
+    <col min="2302" max="2302" width="7.28515625" style="4" customWidth="1"/>
+    <col min="2303" max="2303" width="17" style="4" customWidth="1"/>
+    <col min="2304" max="2304" width="25.28515625" style="4" customWidth="1"/>
+    <col min="2305" max="2305" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="8" style="4" customWidth="1"/>
+    <col min="2307" max="2307" width="18.85546875" style="4" customWidth="1"/>
+    <col min="2308" max="2308" width="7.28515625" style="4" customWidth="1"/>
+    <col min="2309" max="2311" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="2312" max="2557" width="9.140625" style="4"/>
+    <col min="2558" max="2558" width="7.28515625" style="4" customWidth="1"/>
+    <col min="2559" max="2559" width="17" style="4" customWidth="1"/>
+    <col min="2560" max="2560" width="25.28515625" style="4" customWidth="1"/>
+    <col min="2561" max="2561" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="8" style="4" customWidth="1"/>
+    <col min="2563" max="2563" width="18.85546875" style="4" customWidth="1"/>
+    <col min="2564" max="2564" width="7.28515625" style="4" customWidth="1"/>
+    <col min="2565" max="2567" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="2568" max="2813" width="9.140625" style="4"/>
+    <col min="2814" max="2814" width="7.28515625" style="4" customWidth="1"/>
+    <col min="2815" max="2815" width="17" style="4" customWidth="1"/>
+    <col min="2816" max="2816" width="25.28515625" style="4" customWidth="1"/>
+    <col min="2817" max="2817" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="8" style="4" customWidth="1"/>
+    <col min="2819" max="2819" width="18.85546875" style="4" customWidth="1"/>
+    <col min="2820" max="2820" width="7.28515625" style="4" customWidth="1"/>
+    <col min="2821" max="2823" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="2824" max="3069" width="9.140625" style="4"/>
+    <col min="3070" max="3070" width="7.28515625" style="4" customWidth="1"/>
+    <col min="3071" max="3071" width="17" style="4" customWidth="1"/>
+    <col min="3072" max="3072" width="25.28515625" style="4" customWidth="1"/>
+    <col min="3073" max="3073" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="8" style="4" customWidth="1"/>
+    <col min="3075" max="3075" width="18.85546875" style="4" customWidth="1"/>
+    <col min="3076" max="3076" width="7.28515625" style="4" customWidth="1"/>
+    <col min="3077" max="3079" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="3080" max="3325" width="9.140625" style="4"/>
+    <col min="3326" max="3326" width="7.28515625" style="4" customWidth="1"/>
+    <col min="3327" max="3327" width="17" style="4" customWidth="1"/>
+    <col min="3328" max="3328" width="25.28515625" style="4" customWidth="1"/>
+    <col min="3329" max="3329" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="8" style="4" customWidth="1"/>
+    <col min="3331" max="3331" width="18.85546875" style="4" customWidth="1"/>
+    <col min="3332" max="3332" width="7.28515625" style="4" customWidth="1"/>
+    <col min="3333" max="3335" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="3336" max="3581" width="9.140625" style="4"/>
+    <col min="3582" max="3582" width="7.28515625" style="4" customWidth="1"/>
+    <col min="3583" max="3583" width="17" style="4" customWidth="1"/>
+    <col min="3584" max="3584" width="25.28515625" style="4" customWidth="1"/>
+    <col min="3585" max="3585" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="8" style="4" customWidth="1"/>
+    <col min="3587" max="3587" width="18.85546875" style="4" customWidth="1"/>
+    <col min="3588" max="3588" width="7.28515625" style="4" customWidth="1"/>
+    <col min="3589" max="3591" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="3592" max="3837" width="9.140625" style="4"/>
+    <col min="3838" max="3838" width="7.28515625" style="4" customWidth="1"/>
+    <col min="3839" max="3839" width="17" style="4" customWidth="1"/>
+    <col min="3840" max="3840" width="25.28515625" style="4" customWidth="1"/>
+    <col min="3841" max="3841" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="8" style="4" customWidth="1"/>
+    <col min="3843" max="3843" width="18.85546875" style="4" customWidth="1"/>
+    <col min="3844" max="3844" width="7.28515625" style="4" customWidth="1"/>
+    <col min="3845" max="3847" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="3848" max="4093" width="9.140625" style="4"/>
+    <col min="4094" max="4094" width="7.28515625" style="4" customWidth="1"/>
+    <col min="4095" max="4095" width="17" style="4" customWidth="1"/>
+    <col min="4096" max="4096" width="25.28515625" style="4" customWidth="1"/>
+    <col min="4097" max="4097" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="8" style="4" customWidth="1"/>
+    <col min="4099" max="4099" width="18.85546875" style="4" customWidth="1"/>
+    <col min="4100" max="4100" width="7.28515625" style="4" customWidth="1"/>
+    <col min="4101" max="4103" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="4104" max="4349" width="9.140625" style="4"/>
+    <col min="4350" max="4350" width="7.28515625" style="4" customWidth="1"/>
+    <col min="4351" max="4351" width="17" style="4" customWidth="1"/>
+    <col min="4352" max="4352" width="25.28515625" style="4" customWidth="1"/>
+    <col min="4353" max="4353" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="8" style="4" customWidth="1"/>
+    <col min="4355" max="4355" width="18.85546875" style="4" customWidth="1"/>
+    <col min="4356" max="4356" width="7.28515625" style="4" customWidth="1"/>
+    <col min="4357" max="4359" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="4360" max="4605" width="9.140625" style="4"/>
+    <col min="4606" max="4606" width="7.28515625" style="4" customWidth="1"/>
+    <col min="4607" max="4607" width="17" style="4" customWidth="1"/>
+    <col min="4608" max="4608" width="25.28515625" style="4" customWidth="1"/>
+    <col min="4609" max="4609" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="8" style="4" customWidth="1"/>
+    <col min="4611" max="4611" width="18.85546875" style="4" customWidth="1"/>
+    <col min="4612" max="4612" width="7.28515625" style="4" customWidth="1"/>
+    <col min="4613" max="4615" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="4616" max="4861" width="9.140625" style="4"/>
+    <col min="4862" max="4862" width="7.28515625" style="4" customWidth="1"/>
+    <col min="4863" max="4863" width="17" style="4" customWidth="1"/>
+    <col min="4864" max="4864" width="25.28515625" style="4" customWidth="1"/>
+    <col min="4865" max="4865" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="8" style="4" customWidth="1"/>
+    <col min="4867" max="4867" width="18.85546875" style="4" customWidth="1"/>
+    <col min="4868" max="4868" width="7.28515625" style="4" customWidth="1"/>
+    <col min="4869" max="4871" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="4872" max="5117" width="9.140625" style="4"/>
+    <col min="5118" max="5118" width="7.28515625" style="4" customWidth="1"/>
+    <col min="5119" max="5119" width="17" style="4" customWidth="1"/>
+    <col min="5120" max="5120" width="25.28515625" style="4" customWidth="1"/>
+    <col min="5121" max="5121" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="8" style="4" customWidth="1"/>
+    <col min="5123" max="5123" width="18.85546875" style="4" customWidth="1"/>
+    <col min="5124" max="5124" width="7.28515625" style="4" customWidth="1"/>
+    <col min="5125" max="5127" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="5128" max="5373" width="9.140625" style="4"/>
+    <col min="5374" max="5374" width="7.28515625" style="4" customWidth="1"/>
+    <col min="5375" max="5375" width="17" style="4" customWidth="1"/>
+    <col min="5376" max="5376" width="25.28515625" style="4" customWidth="1"/>
+    <col min="5377" max="5377" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="8" style="4" customWidth="1"/>
+    <col min="5379" max="5379" width="18.85546875" style="4" customWidth="1"/>
+    <col min="5380" max="5380" width="7.28515625" style="4" customWidth="1"/>
+    <col min="5381" max="5383" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="5384" max="5629" width="9.140625" style="4"/>
+    <col min="5630" max="5630" width="7.28515625" style="4" customWidth="1"/>
+    <col min="5631" max="5631" width="17" style="4" customWidth="1"/>
+    <col min="5632" max="5632" width="25.28515625" style="4" customWidth="1"/>
+    <col min="5633" max="5633" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="8" style="4" customWidth="1"/>
+    <col min="5635" max="5635" width="18.85546875" style="4" customWidth="1"/>
+    <col min="5636" max="5636" width="7.28515625" style="4" customWidth="1"/>
+    <col min="5637" max="5639" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="5640" max="5885" width="9.140625" style="4"/>
+    <col min="5886" max="5886" width="7.28515625" style="4" customWidth="1"/>
+    <col min="5887" max="5887" width="17" style="4" customWidth="1"/>
+    <col min="5888" max="5888" width="25.28515625" style="4" customWidth="1"/>
+    <col min="5889" max="5889" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="8" style="4" customWidth="1"/>
+    <col min="5891" max="5891" width="18.85546875" style="4" customWidth="1"/>
+    <col min="5892" max="5892" width="7.28515625" style="4" customWidth="1"/>
+    <col min="5893" max="5895" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="5896" max="6141" width="9.140625" style="4"/>
+    <col min="6142" max="6142" width="7.28515625" style="4" customWidth="1"/>
+    <col min="6143" max="6143" width="17" style="4" customWidth="1"/>
+    <col min="6144" max="6144" width="25.28515625" style="4" customWidth="1"/>
+    <col min="6145" max="6145" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="8" style="4" customWidth="1"/>
+    <col min="6147" max="6147" width="18.85546875" style="4" customWidth="1"/>
+    <col min="6148" max="6148" width="7.28515625" style="4" customWidth="1"/>
+    <col min="6149" max="6151" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="6152" max="6397" width="9.140625" style="4"/>
+    <col min="6398" max="6398" width="7.28515625" style="4" customWidth="1"/>
+    <col min="6399" max="6399" width="17" style="4" customWidth="1"/>
+    <col min="6400" max="6400" width="25.28515625" style="4" customWidth="1"/>
+    <col min="6401" max="6401" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="8" style="4" customWidth="1"/>
+    <col min="6403" max="6403" width="18.85546875" style="4" customWidth="1"/>
+    <col min="6404" max="6404" width="7.28515625" style="4" customWidth="1"/>
+    <col min="6405" max="6407" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="6408" max="6653" width="9.140625" style="4"/>
+    <col min="6654" max="6654" width="7.28515625" style="4" customWidth="1"/>
+    <col min="6655" max="6655" width="17" style="4" customWidth="1"/>
+    <col min="6656" max="6656" width="25.28515625" style="4" customWidth="1"/>
+    <col min="6657" max="6657" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="8" style="4" customWidth="1"/>
+    <col min="6659" max="6659" width="18.85546875" style="4" customWidth="1"/>
+    <col min="6660" max="6660" width="7.28515625" style="4" customWidth="1"/>
+    <col min="6661" max="6663" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="6664" max="6909" width="9.140625" style="4"/>
+    <col min="6910" max="6910" width="7.28515625" style="4" customWidth="1"/>
+    <col min="6911" max="6911" width="17" style="4" customWidth="1"/>
+    <col min="6912" max="6912" width="25.28515625" style="4" customWidth="1"/>
+    <col min="6913" max="6913" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="8" style="4" customWidth="1"/>
+    <col min="6915" max="6915" width="18.85546875" style="4" customWidth="1"/>
+    <col min="6916" max="6916" width="7.28515625" style="4" customWidth="1"/>
+    <col min="6917" max="6919" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="6920" max="7165" width="9.140625" style="4"/>
+    <col min="7166" max="7166" width="7.28515625" style="4" customWidth="1"/>
+    <col min="7167" max="7167" width="17" style="4" customWidth="1"/>
+    <col min="7168" max="7168" width="25.28515625" style="4" customWidth="1"/>
+    <col min="7169" max="7169" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="8" style="4" customWidth="1"/>
+    <col min="7171" max="7171" width="18.85546875" style="4" customWidth="1"/>
+    <col min="7172" max="7172" width="7.28515625" style="4" customWidth="1"/>
+    <col min="7173" max="7175" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="7176" max="7421" width="9.140625" style="4"/>
+    <col min="7422" max="7422" width="7.28515625" style="4" customWidth="1"/>
+    <col min="7423" max="7423" width="17" style="4" customWidth="1"/>
+    <col min="7424" max="7424" width="25.28515625" style="4" customWidth="1"/>
+    <col min="7425" max="7425" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="8" style="4" customWidth="1"/>
+    <col min="7427" max="7427" width="18.85546875" style="4" customWidth="1"/>
+    <col min="7428" max="7428" width="7.28515625" style="4" customWidth="1"/>
+    <col min="7429" max="7431" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="7432" max="7677" width="9.140625" style="4"/>
+    <col min="7678" max="7678" width="7.28515625" style="4" customWidth="1"/>
+    <col min="7679" max="7679" width="17" style="4" customWidth="1"/>
+    <col min="7680" max="7680" width="25.28515625" style="4" customWidth="1"/>
+    <col min="7681" max="7681" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="8" style="4" customWidth="1"/>
+    <col min="7683" max="7683" width="18.85546875" style="4" customWidth="1"/>
+    <col min="7684" max="7684" width="7.28515625" style="4" customWidth="1"/>
+    <col min="7685" max="7687" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="7688" max="7933" width="9.140625" style="4"/>
+    <col min="7934" max="7934" width="7.28515625" style="4" customWidth="1"/>
+    <col min="7935" max="7935" width="17" style="4" customWidth="1"/>
+    <col min="7936" max="7936" width="25.28515625" style="4" customWidth="1"/>
+    <col min="7937" max="7937" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="8" style="4" customWidth="1"/>
+    <col min="7939" max="7939" width="18.85546875" style="4" customWidth="1"/>
+    <col min="7940" max="7940" width="7.28515625" style="4" customWidth="1"/>
+    <col min="7941" max="7943" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="7944" max="8189" width="9.140625" style="4"/>
+    <col min="8190" max="8190" width="7.28515625" style="4" customWidth="1"/>
+    <col min="8191" max="8191" width="17" style="4" customWidth="1"/>
+    <col min="8192" max="8192" width="25.28515625" style="4" customWidth="1"/>
+    <col min="8193" max="8193" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="8" style="4" customWidth="1"/>
+    <col min="8195" max="8195" width="18.85546875" style="4" customWidth="1"/>
+    <col min="8196" max="8196" width="7.28515625" style="4" customWidth="1"/>
+    <col min="8197" max="8199" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="8200" max="8445" width="9.140625" style="4"/>
+    <col min="8446" max="8446" width="7.28515625" style="4" customWidth="1"/>
+    <col min="8447" max="8447" width="17" style="4" customWidth="1"/>
+    <col min="8448" max="8448" width="25.28515625" style="4" customWidth="1"/>
+    <col min="8449" max="8449" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="8" style="4" customWidth="1"/>
+    <col min="8451" max="8451" width="18.85546875" style="4" customWidth="1"/>
+    <col min="8452" max="8452" width="7.28515625" style="4" customWidth="1"/>
+    <col min="8453" max="8455" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="8456" max="8701" width="9.140625" style="4"/>
+    <col min="8702" max="8702" width="7.28515625" style="4" customWidth="1"/>
+    <col min="8703" max="8703" width="17" style="4" customWidth="1"/>
+    <col min="8704" max="8704" width="25.28515625" style="4" customWidth="1"/>
+    <col min="8705" max="8705" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="8" style="4" customWidth="1"/>
+    <col min="8707" max="8707" width="18.85546875" style="4" customWidth="1"/>
+    <col min="8708" max="8708" width="7.28515625" style="4" customWidth="1"/>
+    <col min="8709" max="8711" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="8712" max="8957" width="9.140625" style="4"/>
+    <col min="8958" max="8958" width="7.28515625" style="4" customWidth="1"/>
+    <col min="8959" max="8959" width="17" style="4" customWidth="1"/>
+    <col min="8960" max="8960" width="25.28515625" style="4" customWidth="1"/>
+    <col min="8961" max="8961" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="8" style="4" customWidth="1"/>
+    <col min="8963" max="8963" width="18.85546875" style="4" customWidth="1"/>
+    <col min="8964" max="8964" width="7.28515625" style="4" customWidth="1"/>
+    <col min="8965" max="8967" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="8968" max="9213" width="9.140625" style="4"/>
+    <col min="9214" max="9214" width="7.28515625" style="4" customWidth="1"/>
+    <col min="9215" max="9215" width="17" style="4" customWidth="1"/>
+    <col min="9216" max="9216" width="25.28515625" style="4" customWidth="1"/>
+    <col min="9217" max="9217" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="8" style="4" customWidth="1"/>
+    <col min="9219" max="9219" width="18.85546875" style="4" customWidth="1"/>
+    <col min="9220" max="9220" width="7.28515625" style="4" customWidth="1"/>
+    <col min="9221" max="9223" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="9224" max="9469" width="9.140625" style="4"/>
+    <col min="9470" max="9470" width="7.28515625" style="4" customWidth="1"/>
+    <col min="9471" max="9471" width="17" style="4" customWidth="1"/>
+    <col min="9472" max="9472" width="25.28515625" style="4" customWidth="1"/>
+    <col min="9473" max="9473" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="8" style="4" customWidth="1"/>
+    <col min="9475" max="9475" width="18.85546875" style="4" customWidth="1"/>
+    <col min="9476" max="9476" width="7.28515625" style="4" customWidth="1"/>
+    <col min="9477" max="9479" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="9480" max="9725" width="9.140625" style="4"/>
+    <col min="9726" max="9726" width="7.28515625" style="4" customWidth="1"/>
+    <col min="9727" max="9727" width="17" style="4" customWidth="1"/>
+    <col min="9728" max="9728" width="25.28515625" style="4" customWidth="1"/>
+    <col min="9729" max="9729" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="8" style="4" customWidth="1"/>
+    <col min="9731" max="9731" width="18.85546875" style="4" customWidth="1"/>
+    <col min="9732" max="9732" width="7.28515625" style="4" customWidth="1"/>
+    <col min="9733" max="9735" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="9736" max="9981" width="9.140625" style="4"/>
+    <col min="9982" max="9982" width="7.28515625" style="4" customWidth="1"/>
+    <col min="9983" max="9983" width="17" style="4" customWidth="1"/>
+    <col min="9984" max="9984" width="25.28515625" style="4" customWidth="1"/>
+    <col min="9985" max="9985" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="8" style="4" customWidth="1"/>
+    <col min="9987" max="9987" width="18.85546875" style="4" customWidth="1"/>
+    <col min="9988" max="9988" width="7.28515625" style="4" customWidth="1"/>
+    <col min="9989" max="9991" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="9992" max="10237" width="9.140625" style="4"/>
+    <col min="10238" max="10238" width="7.28515625" style="4" customWidth="1"/>
+    <col min="10239" max="10239" width="17" style="4" customWidth="1"/>
+    <col min="10240" max="10240" width="25.28515625" style="4" customWidth="1"/>
+    <col min="10241" max="10241" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="8" style="4" customWidth="1"/>
+    <col min="10243" max="10243" width="18.85546875" style="4" customWidth="1"/>
+    <col min="10244" max="10244" width="7.28515625" style="4" customWidth="1"/>
+    <col min="10245" max="10247" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="10248" max="10493" width="9.140625" style="4"/>
+    <col min="10494" max="10494" width="7.28515625" style="4" customWidth="1"/>
+    <col min="10495" max="10495" width="17" style="4" customWidth="1"/>
+    <col min="10496" max="10496" width="25.28515625" style="4" customWidth="1"/>
+    <col min="10497" max="10497" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="8" style="4" customWidth="1"/>
+    <col min="10499" max="10499" width="18.85546875" style="4" customWidth="1"/>
+    <col min="10500" max="10500" width="7.28515625" style="4" customWidth="1"/>
+    <col min="10501" max="10503" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="10504" max="10749" width="9.140625" style="4"/>
+    <col min="10750" max="10750" width="7.28515625" style="4" customWidth="1"/>
+    <col min="10751" max="10751" width="17" style="4" customWidth="1"/>
+    <col min="10752" max="10752" width="25.28515625" style="4" customWidth="1"/>
+    <col min="10753" max="10753" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="8" style="4" customWidth="1"/>
+    <col min="10755" max="10755" width="18.85546875" style="4" customWidth="1"/>
+    <col min="10756" max="10756" width="7.28515625" style="4" customWidth="1"/>
+    <col min="10757" max="10759" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="10760" max="11005" width="9.140625" style="4"/>
+    <col min="11006" max="11006" width="7.28515625" style="4" customWidth="1"/>
+    <col min="11007" max="11007" width="17" style="4" customWidth="1"/>
+    <col min="11008" max="11008" width="25.28515625" style="4" customWidth="1"/>
+    <col min="11009" max="11009" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="8" style="4" customWidth="1"/>
+    <col min="11011" max="11011" width="18.85546875" style="4" customWidth="1"/>
+    <col min="11012" max="11012" width="7.28515625" style="4" customWidth="1"/>
+    <col min="11013" max="11015" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="11016" max="11261" width="9.140625" style="4"/>
+    <col min="11262" max="11262" width="7.28515625" style="4" customWidth="1"/>
+    <col min="11263" max="11263" width="17" style="4" customWidth="1"/>
+    <col min="11264" max="11264" width="25.28515625" style="4" customWidth="1"/>
+    <col min="11265" max="11265" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="8" style="4" customWidth="1"/>
+    <col min="11267" max="11267" width="18.85546875" style="4" customWidth="1"/>
+    <col min="11268" max="11268" width="7.28515625" style="4" customWidth="1"/>
+    <col min="11269" max="11271" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="11272" max="11517" width="9.140625" style="4"/>
+    <col min="11518" max="11518" width="7.28515625" style="4" customWidth="1"/>
+    <col min="11519" max="11519" width="17" style="4" customWidth="1"/>
+    <col min="11520" max="11520" width="25.28515625" style="4" customWidth="1"/>
+    <col min="11521" max="11521" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="8" style="4" customWidth="1"/>
+    <col min="11523" max="11523" width="18.85546875" style="4" customWidth="1"/>
+    <col min="11524" max="11524" width="7.28515625" style="4" customWidth="1"/>
+    <col min="11525" max="11527" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="11528" max="11773" width="9.140625" style="4"/>
+    <col min="11774" max="11774" width="7.28515625" style="4" customWidth="1"/>
+    <col min="11775" max="11775" width="17" style="4" customWidth="1"/>
+    <col min="11776" max="11776" width="25.28515625" style="4" customWidth="1"/>
+    <col min="11777" max="11777" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="8" style="4" customWidth="1"/>
+    <col min="11779" max="11779" width="18.85546875" style="4" customWidth="1"/>
+    <col min="11780" max="11780" width="7.28515625" style="4" customWidth="1"/>
+    <col min="11781" max="11783" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="11784" max="12029" width="9.140625" style="4"/>
+    <col min="12030" max="12030" width="7.28515625" style="4" customWidth="1"/>
+    <col min="12031" max="12031" width="17" style="4" customWidth="1"/>
+    <col min="12032" max="12032" width="25.28515625" style="4" customWidth="1"/>
+    <col min="12033" max="12033" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="8" style="4" customWidth="1"/>
+    <col min="12035" max="12035" width="18.85546875" style="4" customWidth="1"/>
+    <col min="12036" max="12036" width="7.28515625" style="4" customWidth="1"/>
+    <col min="12037" max="12039" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="12040" max="12285" width="9.140625" style="4"/>
+    <col min="12286" max="12286" width="7.28515625" style="4" customWidth="1"/>
+    <col min="12287" max="12287" width="17" style="4" customWidth="1"/>
+    <col min="12288" max="12288" width="25.28515625" style="4" customWidth="1"/>
+    <col min="12289" max="12289" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="8" style="4" customWidth="1"/>
+    <col min="12291" max="12291" width="18.85546875" style="4" customWidth="1"/>
+    <col min="12292" max="12292" width="7.28515625" style="4" customWidth="1"/>
+    <col min="12293" max="12295" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="12296" max="12541" width="9.140625" style="4"/>
+    <col min="12542" max="12542" width="7.28515625" style="4" customWidth="1"/>
+    <col min="12543" max="12543" width="17" style="4" customWidth="1"/>
+    <col min="12544" max="12544" width="25.28515625" style="4" customWidth="1"/>
+    <col min="12545" max="12545" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="8" style="4" customWidth="1"/>
+    <col min="12547" max="12547" width="18.85546875" style="4" customWidth="1"/>
+    <col min="12548" max="12548" width="7.28515625" style="4" customWidth="1"/>
+    <col min="12549" max="12551" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="12552" max="12797" width="9.140625" style="4"/>
+    <col min="12798" max="12798" width="7.28515625" style="4" customWidth="1"/>
+    <col min="12799" max="12799" width="17" style="4" customWidth="1"/>
+    <col min="12800" max="12800" width="25.28515625" style="4" customWidth="1"/>
+    <col min="12801" max="12801" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="8" style="4" customWidth="1"/>
+    <col min="12803" max="12803" width="18.85546875" style="4" customWidth="1"/>
+    <col min="12804" max="12804" width="7.28515625" style="4" customWidth="1"/>
+    <col min="12805" max="12807" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="12808" max="13053" width="9.140625" style="4"/>
+    <col min="13054" max="13054" width="7.28515625" style="4" customWidth="1"/>
+    <col min="13055" max="13055" width="17" style="4" customWidth="1"/>
+    <col min="13056" max="13056" width="25.28515625" style="4" customWidth="1"/>
+    <col min="13057" max="13057" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="8" style="4" customWidth="1"/>
+    <col min="13059" max="13059" width="18.85546875" style="4" customWidth="1"/>
+    <col min="13060" max="13060" width="7.28515625" style="4" customWidth="1"/>
+    <col min="13061" max="13063" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="13064" max="13309" width="9.140625" style="4"/>
+    <col min="13310" max="13310" width="7.28515625" style="4" customWidth="1"/>
+    <col min="13311" max="13311" width="17" style="4" customWidth="1"/>
+    <col min="13312" max="13312" width="25.28515625" style="4" customWidth="1"/>
+    <col min="13313" max="13313" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="8" style="4" customWidth="1"/>
+    <col min="13315" max="13315" width="18.85546875" style="4" customWidth="1"/>
+    <col min="13316" max="13316" width="7.28515625" style="4" customWidth="1"/>
+    <col min="13317" max="13319" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="13320" max="13565" width="9.140625" style="4"/>
+    <col min="13566" max="13566" width="7.28515625" style="4" customWidth="1"/>
+    <col min="13567" max="13567" width="17" style="4" customWidth="1"/>
+    <col min="13568" max="13568" width="25.28515625" style="4" customWidth="1"/>
+    <col min="13569" max="13569" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="8" style="4" customWidth="1"/>
+    <col min="13571" max="13571" width="18.85546875" style="4" customWidth="1"/>
+    <col min="13572" max="13572" width="7.28515625" style="4" customWidth="1"/>
+    <col min="13573" max="13575" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="13576" max="13821" width="9.140625" style="4"/>
+    <col min="13822" max="13822" width="7.28515625" style="4" customWidth="1"/>
+    <col min="13823" max="13823" width="17" style="4" customWidth="1"/>
+    <col min="13824" max="13824" width="25.28515625" style="4" customWidth="1"/>
+    <col min="13825" max="13825" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="8" style="4" customWidth="1"/>
+    <col min="13827" max="13827" width="18.85546875" style="4" customWidth="1"/>
+    <col min="13828" max="13828" width="7.28515625" style="4" customWidth="1"/>
+    <col min="13829" max="13831" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="13832" max="14077" width="9.140625" style="4"/>
+    <col min="14078" max="14078" width="7.28515625" style="4" customWidth="1"/>
+    <col min="14079" max="14079" width="17" style="4" customWidth="1"/>
+    <col min="14080" max="14080" width="25.28515625" style="4" customWidth="1"/>
+    <col min="14081" max="14081" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="8" style="4" customWidth="1"/>
+    <col min="14083" max="14083" width="18.85546875" style="4" customWidth="1"/>
+    <col min="14084" max="14084" width="7.28515625" style="4" customWidth="1"/>
+    <col min="14085" max="14087" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="14088" max="14333" width="9.140625" style="4"/>
+    <col min="14334" max="14334" width="7.28515625" style="4" customWidth="1"/>
+    <col min="14335" max="14335" width="17" style="4" customWidth="1"/>
+    <col min="14336" max="14336" width="25.28515625" style="4" customWidth="1"/>
+    <col min="14337" max="14337" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="8" style="4" customWidth="1"/>
+    <col min="14339" max="14339" width="18.85546875" style="4" customWidth="1"/>
+    <col min="14340" max="14340" width="7.28515625" style="4" customWidth="1"/>
+    <col min="14341" max="14343" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="14344" max="14589" width="9.140625" style="4"/>
+    <col min="14590" max="14590" width="7.28515625" style="4" customWidth="1"/>
+    <col min="14591" max="14591" width="17" style="4" customWidth="1"/>
+    <col min="14592" max="14592" width="25.28515625" style="4" customWidth="1"/>
+    <col min="14593" max="14593" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="8" style="4" customWidth="1"/>
+    <col min="14595" max="14595" width="18.85546875" style="4" customWidth="1"/>
+    <col min="14596" max="14596" width="7.28515625" style="4" customWidth="1"/>
+    <col min="14597" max="14599" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="14600" max="14845" width="9.140625" style="4"/>
+    <col min="14846" max="14846" width="7.28515625" style="4" customWidth="1"/>
+    <col min="14847" max="14847" width="17" style="4" customWidth="1"/>
+    <col min="14848" max="14848" width="25.28515625" style="4" customWidth="1"/>
+    <col min="14849" max="14849" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="8" style="4" customWidth="1"/>
+    <col min="14851" max="14851" width="18.85546875" style="4" customWidth="1"/>
+    <col min="14852" max="14852" width="7.28515625" style="4" customWidth="1"/>
+    <col min="14853" max="14855" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="14856" max="15101" width="9.140625" style="4"/>
+    <col min="15102" max="15102" width="7.28515625" style="4" customWidth="1"/>
+    <col min="15103" max="15103" width="17" style="4" customWidth="1"/>
+    <col min="15104" max="15104" width="25.28515625" style="4" customWidth="1"/>
+    <col min="15105" max="15105" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="8" style="4" customWidth="1"/>
+    <col min="15107" max="15107" width="18.85546875" style="4" customWidth="1"/>
+    <col min="15108" max="15108" width="7.28515625" style="4" customWidth="1"/>
+    <col min="15109" max="15111" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="15112" max="15357" width="9.140625" style="4"/>
+    <col min="15358" max="15358" width="7.28515625" style="4" customWidth="1"/>
+    <col min="15359" max="15359" width="17" style="4" customWidth="1"/>
+    <col min="15360" max="15360" width="25.28515625" style="4" customWidth="1"/>
+    <col min="15361" max="15361" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="8" style="4" customWidth="1"/>
+    <col min="15363" max="15363" width="18.85546875" style="4" customWidth="1"/>
+    <col min="15364" max="15364" width="7.28515625" style="4" customWidth="1"/>
+    <col min="15365" max="15367" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="15368" max="15613" width="9.140625" style="4"/>
+    <col min="15614" max="15614" width="7.28515625" style="4" customWidth="1"/>
+    <col min="15615" max="15615" width="17" style="4" customWidth="1"/>
+    <col min="15616" max="15616" width="25.28515625" style="4" customWidth="1"/>
+    <col min="15617" max="15617" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="8" style="4" customWidth="1"/>
+    <col min="15619" max="15619" width="18.85546875" style="4" customWidth="1"/>
+    <col min="15620" max="15620" width="7.28515625" style="4" customWidth="1"/>
+    <col min="15621" max="15623" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="15624" max="15869" width="9.140625" style="4"/>
+    <col min="15870" max="15870" width="7.28515625" style="4" customWidth="1"/>
+    <col min="15871" max="15871" width="17" style="4" customWidth="1"/>
+    <col min="15872" max="15872" width="25.28515625" style="4" customWidth="1"/>
+    <col min="15873" max="15873" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="8" style="4" customWidth="1"/>
+    <col min="15875" max="15875" width="18.85546875" style="4" customWidth="1"/>
+    <col min="15876" max="15876" width="7.28515625" style="4" customWidth="1"/>
+    <col min="15877" max="15879" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="15880" max="16125" width="9.140625" style="4"/>
+    <col min="16126" max="16126" width="7.28515625" style="4" customWidth="1"/>
+    <col min="16127" max="16127" width="17" style="4" customWidth="1"/>
+    <col min="16128" max="16128" width="25.28515625" style="4" customWidth="1"/>
+    <col min="16129" max="16129" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="8" style="4" customWidth="1"/>
+    <col min="16131" max="16131" width="18.85546875" style="4" customWidth="1"/>
+    <col min="16132" max="16132" width="7.28515625" style="4" customWidth="1"/>
+    <col min="16133" max="16135" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="16136" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16138" ht="15" customHeight="1">
-      <c r="C1" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16138" ht="15" customHeight="1">
-      <c r="A2" s="6" t="s">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>12</v>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
       </c>
-      <c r="E2" s="29"/>
-    </row>
-    <row r="3" spans="1:16138" ht="15" customHeight="1">
-      <c r="A3" s="12" t="s">
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="24"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="1:16138" ht="18.75" customHeight="1">
+      <c r="E3" s="7"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -5735,561 +5678,276 @@
       <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>7</v>
+      <c r="H4" s="3" t="s">
+        <v>24</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F5" s="10"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-    </row>
-    <row r="6" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F6" s="32"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F7" s="10"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F8" s="10"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F9" s="15"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="31"/>
-      <c r="B10" s="29"/>
-      <c r="F10" s="10"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F11" s="10"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F12" s="10"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F13" s="10"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F14" s="10"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F15" s="10"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F16" s="10"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F17" s="10"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F18" s="10"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F19" s="10"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F20" s="10"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F21" s="10"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-    </row>
-    <row r="22" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F22" s="10"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-    </row>
-    <row r="23" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F23" s="10"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F24" s="10"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F25" s="10"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F26" s="10"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F27" s="10"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-    </row>
-    <row r="28" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F28" s="10"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F29" s="10"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F30" s="10"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-    </row>
-    <row r="31" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F31" s="10"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F32" s="10"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-    </row>
-    <row r="33" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F33" s="10"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-    </row>
-    <row r="34" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F34" s="10"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-    </row>
-    <row r="35" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F35" s="10"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-    </row>
-    <row r="36" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F36" s="10"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-    </row>
-    <row r="37" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F37" s="10"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-    </row>
-    <row r="38" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F38" s="10"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-    </row>
-    <row r="39" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F39" s="10"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-    </row>
-    <row r="40" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F40" s="10"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
-    </row>
-    <row r="41" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F41" s="10"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-    </row>
-    <row r="42" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F42" s="10"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
-    </row>
-    <row r="43" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F43" s="10"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-    </row>
-    <row r="44" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F44" s="10"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-    </row>
-    <row r="45" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F45" s="10"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-    </row>
-    <row r="46" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F46" s="10"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-    </row>
-    <row r="47" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F47" s="10"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-    </row>
-    <row r="48" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F48" s="10"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-    </row>
-    <row r="49" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F49" s="10"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-    </row>
-    <row r="50" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F50" s="10"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-    </row>
-    <row r="51" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F51" s="10"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-    </row>
-    <row r="52" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F52" s="10"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-    </row>
-    <row r="53" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F53" s="10"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
-    </row>
-    <row r="54" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F54" s="10"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-    </row>
-    <row r="55" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F55" s="10"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-    </row>
-    <row r="56" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F56" s="10"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
-    </row>
-    <row r="57" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F57" s="10"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-    </row>
-    <row r="58" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F58" s="10"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9"/>
-    </row>
-    <row r="59" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F59" s="10"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
-    </row>
-    <row r="60" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F60" s="10"/>
-      <c r="H60" s="7"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="9"/>
-    </row>
-    <row r="61" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F61" s="10"/>
-      <c r="H61" s="7"/>
-      <c r="I61" s="9"/>
-      <c r="J61" s="9"/>
-    </row>
-    <row r="62" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F62" s="10"/>
-      <c r="H62" s="7"/>
-      <c r="I62" s="9"/>
-      <c r="J62" s="9"/>
-    </row>
-    <row r="63" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F63" s="10"/>
-      <c r="H63" s="7"/>
-      <c r="I63" s="9"/>
-      <c r="J63" s="9"/>
-    </row>
-    <row r="64" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F64" s="10"/>
-      <c r="H64" s="7"/>
-      <c r="I64" s="9"/>
-      <c r="J64" s="9"/>
-    </row>
-    <row r="65" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F65" s="10"/>
-      <c r="H65" s="7"/>
-      <c r="I65" s="9"/>
-      <c r="J65" s="9"/>
-    </row>
-    <row r="66" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F66" s="10"/>
-      <c r="H66" s="7"/>
-      <c r="I66" s="9"/>
-      <c r="J66" s="9"/>
-    </row>
-    <row r="67" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F67" s="10"/>
-      <c r="H67" s="7"/>
-      <c r="I67" s="9"/>
-      <c r="J67" s="9"/>
-    </row>
-    <row r="68" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F68" s="10"/>
-      <c r="H68" s="7"/>
-      <c r="I68" s="9"/>
-      <c r="J68" s="9"/>
-    </row>
-    <row r="69" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F69" s="10"/>
-      <c r="H69" s="7"/>
-      <c r="I69" s="9"/>
-      <c r="J69" s="9"/>
-    </row>
-    <row r="70" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F70" s="10"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="9"/>
-      <c r="J70" s="9"/>
-    </row>
-    <row r="71" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F71" s="10"/>
-      <c r="H71" s="7"/>
-      <c r="I71" s="9"/>
-      <c r="J71" s="9"/>
-    </row>
-    <row r="72" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F72" s="10"/>
-      <c r="H72" s="7"/>
-      <c r="I72" s="9"/>
-      <c r="J72" s="9"/>
-    </row>
-    <row r="73" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F73" s="10"/>
-      <c r="H73" s="7"/>
-      <c r="I73" s="9"/>
-      <c r="J73" s="9"/>
-    </row>
-    <row r="74" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F74" s="10"/>
-      <c r="H74" s="7"/>
-      <c r="I74" s="9"/>
-      <c r="J74" s="9"/>
-    </row>
-    <row r="75" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F75" s="10"/>
-      <c r="H75" s="7"/>
-      <c r="I75" s="9"/>
-      <c r="J75" s="9"/>
-    </row>
-    <row r="76" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F76" s="10"/>
-      <c r="H76" s="7"/>
-      <c r="I76" s="9"/>
-      <c r="J76" s="9"/>
-    </row>
-    <row r="77" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F77" s="10"/>
-      <c r="H77" s="7"/>
-      <c r="I77" s="9"/>
-      <c r="J77" s="9"/>
-    </row>
-    <row r="78" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F78" s="10"/>
-      <c r="H78" s="7"/>
-      <c r="I78" s="9"/>
-      <c r="J78" s="9"/>
-    </row>
-    <row r="79" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F79" s="10"/>
-      <c r="H79" s="7"/>
-      <c r="I79" s="9"/>
-      <c r="J79" s="9"/>
-    </row>
-    <row r="80" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F80" s="10"/>
-      <c r="H80" s="7"/>
-      <c r="I80" s="9"/>
-      <c r="J80" s="9"/>
-    </row>
-    <row r="81" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F81" s="10"/>
-      <c r="H81" s="7"/>
-      <c r="I81" s="9"/>
-      <c r="J81" s="9"/>
-    </row>
-    <row r="82" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F82" s="10"/>
-      <c r="H82" s="7"/>
-      <c r="I82" s="9"/>
-      <c r="J82" s="9"/>
-    </row>
-    <row r="83" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F83" s="10"/>
-      <c r="H83" s="7"/>
-      <c r="I83" s="9"/>
-      <c r="J83" s="9"/>
-    </row>
-    <row r="84" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F84" s="10"/>
-      <c r="H84" s="7"/>
-      <c r="I84" s="9"/>
-      <c r="J84" s="9"/>
-    </row>
-    <row r="85" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F85" s="10"/>
-      <c r="H85" s="7"/>
-      <c r="I85" s="9"/>
-      <c r="J85" s="9"/>
-    </row>
-    <row r="86" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F86" s="10"/>
-      <c r="H86" s="7"/>
-      <c r="I86" s="9"/>
-      <c r="J86" s="9"/>
-    </row>
-    <row r="87" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F87" s="10"/>
-      <c r="H87" s="7"/>
-      <c r="I87" s="9"/>
-      <c r="J87" s="9"/>
-    </row>
-    <row r="88" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F88" s="10"/>
-      <c r="H88" s="7"/>
-      <c r="I88" s="9"/>
-      <c r="J88" s="9"/>
-    </row>
-    <row r="89" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F89" s="10"/>
-      <c r="H89" s="7"/>
-      <c r="I89" s="9"/>
-      <c r="J89" s="9"/>
-    </row>
-    <row r="90" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F90" s="10"/>
-      <c r="H90" s="7"/>
-      <c r="I90" s="9"/>
-      <c r="J90" s="9"/>
-    </row>
-    <row r="91" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F91" s="10"/>
-      <c r="H91" s="7"/>
-      <c r="I91" s="9"/>
-      <c r="J91" s="9"/>
-    </row>
-    <row r="92" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="F92" s="10"/>
-      <c r="H92" s="7"/>
-      <c r="I92" s="9"/>
-      <c r="J92" s="9"/>
-    </row>
-    <row r="93" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="94" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="95" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="96" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="97" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="98" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="99" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="100" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="101" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="102" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="103" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="104" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="105" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="106" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="107" spans="1:16138" s="6" customFormat="1" ht="15" customHeight="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1">
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1">
+      <c r="F6" s="27"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1">
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1">
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1">
+      <c r="A10" s="26"/>
+      <c r="B10" s="24"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1">
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1">
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1">
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="6:6" ht="15" customHeight="1">
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="6:6" ht="15" customHeight="1">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="6:6" ht="15" customHeight="1">
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="6:6" ht="15" customHeight="1">
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="6:6" ht="15" customHeight="1">
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="6:6" ht="15" customHeight="1">
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="6:6" ht="15" customHeight="1">
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="6:6" ht="15" customHeight="1">
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="6:6" ht="15" customHeight="1">
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="6:6" ht="15" customHeight="1">
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="6:6" ht="15" customHeight="1">
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="6:6" ht="15" customHeight="1">
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="6:6" ht="15" customHeight="1">
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="6:6" ht="15" customHeight="1">
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="6:6" ht="15" customHeight="1">
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="6:6" ht="15" customHeight="1">
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="6:6" ht="15" customHeight="1">
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="6:6" ht="15" customHeight="1">
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="6:6" ht="15" customHeight="1">
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="6:6" ht="15" customHeight="1">
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="6:6" ht="15" customHeight="1">
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="6:6" ht="15" customHeight="1">
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="6:6" ht="15" customHeight="1">
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="6:6" ht="15" customHeight="1">
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="6:6" ht="15" customHeight="1">
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="6:6" ht="15" customHeight="1">
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="6:6" ht="15" customHeight="1">
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="6:6" ht="15" customHeight="1">
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="6:6" ht="15" customHeight="1">
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="6:6" ht="15" customHeight="1">
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="6:6" ht="15" customHeight="1">
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="6:6" ht="15" customHeight="1">
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="6:6" ht="15" customHeight="1">
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="6:6" ht="15" customHeight="1">
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="6:6" ht="15" customHeight="1">
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="6:6" ht="15" customHeight="1">
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="6:6" ht="15" customHeight="1">
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="6:6" ht="15" customHeight="1">
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="6:6" ht="15" customHeight="1">
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="6:6" ht="15" customHeight="1">
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="6:6" ht="15" customHeight="1">
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" spans="6:6" ht="15" customHeight="1">
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="6:6" ht="15" customHeight="1">
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" spans="6:6" ht="15" customHeight="1">
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" spans="6:6" ht="15" customHeight="1">
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" spans="6:6" ht="15" customHeight="1">
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="6:6" ht="15" customHeight="1">
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" spans="6:6" ht="15" customHeight="1">
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" spans="6:6" ht="15" customHeight="1">
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" spans="6:6" ht="15" customHeight="1">
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="6:6" ht="15" customHeight="1">
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" spans="6:6" ht="15" customHeight="1">
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="6:6" ht="15" customHeight="1">
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="6:6" ht="15" customHeight="1">
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="6:6" ht="15" customHeight="1">
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="6:6" ht="15" customHeight="1">
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="6:6" ht="15" customHeight="1">
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="6:6" ht="15" customHeight="1">
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" spans="6:6" ht="15" customHeight="1">
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" spans="6:6" ht="15" customHeight="1">
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="6:6" ht="15" customHeight="1">
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" spans="6:6" ht="15" customHeight="1">
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" spans="6:6" ht="15" customHeight="1">
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" spans="6:6" ht="15" customHeight="1">
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" spans="6:6" ht="15" customHeight="1">
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" spans="6:6" ht="15" customHeight="1">
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" spans="6:6" ht="15" customHeight="1">
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84" spans="6:6" ht="15" customHeight="1">
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85" spans="6:6" ht="15" customHeight="1">
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86" spans="6:6" ht="15" customHeight="1">
+      <c r="F86" s="5"/>
+    </row>
+    <row r="87" spans="6:6" ht="15" customHeight="1">
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" spans="6:6" ht="15" customHeight="1">
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89" spans="6:6" ht="15" customHeight="1">
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" spans="6:6" ht="15" customHeight="1">
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" spans="6:6" ht="15" customHeight="1">
+      <c r="F91" s="5"/>
+    </row>
+    <row r="92" spans="6:6" ht="15" customHeight="1">
+      <c r="F92" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.16" right="0.11" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6300,8 +5958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6318,545 +5976,545 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="25.5" customHeight="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="29"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="15"/>
+    </row>
+    <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+    </row>
+    <row r="3" spans="1:24" ht="20.100000000000001" customHeight="1">
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+    </row>
+    <row r="4" spans="1:24" ht="33.75" customHeight="1">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+    </row>
+    <row r="5" spans="1:24" ht="29.25" customHeight="1">
+      <c r="A5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17" t="s">
+      <c r="B5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="20"/>
-    </row>
-    <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
+      <c r="C5" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="21"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="18"/>
+    </row>
+    <row r="6" spans="1:24" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="23">
+        <v>1</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+    </row>
+    <row r="7" spans="1:24" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="23">
+        <v>2</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="1:24" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="23">
+        <v>3</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:24" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="23">
+        <v>4</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="1:24" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="23">
+        <v>5</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="1:24" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="23">
+        <v>6</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="1:24" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="23">
+        <v>7</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:24" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="23">
+        <v>8</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="1:24" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="23">
+        <v>9</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:24" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="23">
+        <v>10</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="R15" s="18"/>
+    </row>
+    <row r="16" spans="1:24" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="23">
+        <v>11</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="N16" s="18"/>
+    </row>
+    <row r="17" spans="1:20" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="23">
+        <v>12</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="N17" s="18"/>
+    </row>
+    <row r="18" spans="1:20" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="23">
+        <v>13</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+    </row>
+    <row r="19" spans="1:20" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="23">
         <v>14</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-    </row>
-    <row r="3" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22" t="s">
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+    </row>
+    <row r="20" spans="1:20" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="23">
+        <v>15</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+    </row>
+    <row r="21" spans="1:20" ht="20.25" customHeight="1">
+      <c r="A21" s="23">
+        <v>16</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+    </row>
+    <row r="22" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A22" s="23">
         <v>17</v>
       </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-    </row>
-    <row r="4" spans="1:24" ht="33.75" customHeight="1">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-    </row>
-    <row r="5" spans="1:24" ht="29.25" customHeight="1">
-      <c r="A5" s="24" t="s">
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+    </row>
+    <row r="23" spans="1:20" ht="20.25" customHeight="1">
+      <c r="A23" s="23">
         <v>18</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="T23" s="18"/>
+    </row>
+    <row r="24" spans="1:20" ht="21" customHeight="1">
+      <c r="A24" s="23">
         <v>19</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+    </row>
+    <row r="25" spans="1:20" ht="20.25" customHeight="1">
+      <c r="A25" s="23">
         <v>20</v>
       </c>
-      <c r="D5" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="26"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="23"/>
-    </row>
-    <row r="6" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="28">
-        <v>1</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-    </row>
-    <row r="7" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="28">
-        <v>2</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-    </row>
-    <row r="8" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="28">
-        <v>3</v>
-      </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="23"/>
-    </row>
-    <row r="9" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="28">
-        <v>4</v>
-      </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="23"/>
-    </row>
-    <row r="10" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="28">
-        <v>5</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="23"/>
-    </row>
-    <row r="11" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="28">
-        <v>6</v>
-      </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="23"/>
-    </row>
-    <row r="12" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="28">
-        <v>7</v>
-      </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="23"/>
-    </row>
-    <row r="13" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="28">
-        <v>8</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="23"/>
-    </row>
-    <row r="14" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="28">
-        <v>9</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="23"/>
-    </row>
-    <row r="15" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="28">
-        <v>10</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="R15" s="23"/>
-    </row>
-    <row r="16" spans="1:24" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="28">
-        <v>11</v>
-      </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="N16" s="23"/>
-    </row>
-    <row r="17" spans="1:20" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="28">
-        <v>12</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="N17" s="23"/>
-    </row>
-    <row r="18" spans="1:20" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="28">
-        <v>13</v>
-      </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-    </row>
-    <row r="19" spans="1:20" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="28">
-        <v>14</v>
-      </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-    </row>
-    <row r="20" spans="1:20" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="28">
-        <v>15</v>
-      </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-    </row>
-    <row r="21" spans="1:20" ht="20.25" customHeight="1">
-      <c r="A21" s="28">
-        <v>16</v>
-      </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-    </row>
-    <row r="22" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A22" s="28">
-        <v>17</v>
-      </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-    </row>
-    <row r="23" spans="1:20" ht="20.25" customHeight="1">
-      <c r="A23" s="28">
-        <v>18</v>
-      </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="T23" s="23"/>
-    </row>
-    <row r="24" spans="1:20" ht="21" customHeight="1">
-      <c r="A24" s="28">
-        <v>19</v>
-      </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-    </row>
-    <row r="25" spans="1:20" ht="20.25" customHeight="1">
-      <c r="A25" s="28">
-        <v>20</v>
-      </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
     </row>
     <row r="26" spans="1:20">
-      <c r="A26" s="23"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
     </row>
     <row r="27" spans="1:20">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:20">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="23"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="A32" s="23"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>